<commit_message>
error xml spec by example completed
</commit_message>
<xml_diff>
--- a/DataScraperAnalysis/Spec Examples.xlsx
+++ b/DataScraperAnalysis/Spec Examples.xlsx
@@ -7,8 +7,8 @@
     <workbookView xWindow="240" yWindow="105" windowWidth="15150" windowHeight="8130"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="8" r:id="rId1"/>
-    <sheet name="error codes" sheetId="7" r:id="rId2"/>
+    <sheet name="not sure about this" sheetId="8" r:id="rId1"/>
+    <sheet name="Error Code XML" sheetId="7" r:id="rId2"/>
     <sheet name="credentials" sheetId="1" r:id="rId3"/>
     <sheet name="e-billing registration" sheetId="2" r:id="rId4"/>
     <sheet name="e-billing account update " sheetId="3" r:id="rId5"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="48">
   <si>
     <t xml:space="preserve">Provided Credentials </t>
   </si>
@@ -54,27 +54,6 @@
   </si>
   <si>
     <t>backoff time</t>
-  </si>
-  <si>
-    <t>scenario</t>
-  </si>
-  <si>
-    <t>error code</t>
-  </si>
-  <si>
-    <t>invalid user credentials</t>
-  </si>
-  <si>
-    <t>e-billing account update required</t>
-  </si>
-  <si>
-    <t>billing company site down</t>
-  </si>
-  <si>
-    <t>billing site page error encountered</t>
-  </si>
-  <si>
-    <t>webscraper broken script</t>
   </si>
   <si>
     <r>
@@ -308,21 +287,6 @@
     <t>Notification Message</t>
   </si>
   <si>
-    <t>"InvalidCredentials"</t>
-  </si>
-  <si>
-    <t>"AccountUpdateRequired"</t>
-  </si>
-  <si>
-    <t>"BillingSiteDown"</t>
-  </si>
-  <si>
-    <t>"BillingSitePageError"</t>
-  </si>
-  <si>
-    <t>"UndeterminedError"</t>
-  </si>
-  <si>
     <t>N/A</t>
   </si>
   <si>
@@ -332,12 +296,6 @@
     <t xml:space="preserve">Post Account Status </t>
   </si>
   <si>
-    <t>user not signed up for e-billing</t>
-  </si>
-  <si>
-    <t>"UserNotSignedUpForEbilling"</t>
-  </si>
-  <si>
     <t>Statement Returned</t>
   </si>
   <si>
@@ -357,6 +315,78 @@
   </si>
   <si>
     <t>webscraper  script correct</t>
+  </si>
+  <si>
+    <t>Scraper attempts to scrape with invalid user credentials</t>
+  </si>
+  <si>
+    <t>Error Scenario</t>
+  </si>
+  <si>
+    <t>XML File Content</t>
+  </si>
+  <si>
+    <t>Scraper attempts to scrape with customer that hasn’t signed up for e-billing</t>
+  </si>
+  <si>
+    <t>Scraper attempts to scrape with customer who’s e-billing process required further customer input to complete</t>
+  </si>
+  <si>
+    <t>Scraper attempts to scrape while the billing company website is down</t>
+  </si>
+  <si>
+    <t>Scraper attempts to scrape while e-billing service is unavailable</t>
+  </si>
+  <si>
+    <t>Scraper attempts to scrape with a nonconforming script</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;scrape-session&gt;
+&lt;base-url&gt;www.elen7045.co.za&lt;/base-url&gt;
+&lt;date&gt;01/06/2009&lt;/&gt;
+&lt;time&gt;12:59:34&lt;/time&gt;
+&lt;error&gt;InvalidCredentials&lt;/error&gt;
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;scrape-session&gt;
+&lt;base-url&gt;www.elen7045.co.za&lt;/base-url&gt;
+&lt;date&gt;01/06/2009&lt;/&gt;
+&lt;time&gt;12:59:34&lt;/time&gt;
+&lt;error&gt;UserNotSignedUpForEbilling&lt;/error&gt;
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;scrape-session&gt;
+&lt;base-url&gt;www.elen7045.co.za&lt;/base-url&gt;
+&lt;date&gt;01/06/2009&lt;/&gt;
+&lt;time&gt;12:59:34&lt;/time&gt;
+&lt;error&gt;AccountUpdateRequired&lt;/error&gt;
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;scrape-session&gt;
+&lt;base-url&gt;www.elen7045.co.za&lt;/base-url&gt;
+&lt;date&gt;01/06/2009&lt;/&gt;
+&lt;time&gt;12:59:34&lt;/time&gt;
+&lt;error&gt;BillingSiteDown&lt;/error&gt;
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;scrape-session&gt;
+&lt;base-url&gt;www.elen7045.co.za&lt;/base-url&gt;
+&lt;date&gt;01/06/2009&lt;/&gt;
+&lt;time&gt;12:59:34&lt;/time&gt;
+&lt;error&gt;BillingSitePageError&lt;/error&gt;
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;scrape-session&gt;
+&lt;base-url&gt;www.elen7045.co.za&lt;/base-url&gt;
+&lt;date&gt;01/06/2009&lt;/&gt;
+&lt;time&gt;12:59:34&lt;/time&gt;
+&lt;error&gt;UndeterminedError&lt;/error&gt;
+</t>
   </si>
 </sst>
 </file>
@@ -593,7 +623,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -620,8 +650,19 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -919,7 +960,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection sqref="A1:G5"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -935,25 +976,25 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="G1" s="23" t="s">
-        <v>41</v>
+        <v>33</v>
+      </c>
+      <c r="G1" s="22" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -1068,72 +1109,72 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="32.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="51.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" s="22" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="1" t="s">
+      <c r="A1" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="74.25" customHeight="1">
+      <c r="A2" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="79.5" customHeight="1">
+      <c r="A3" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="25" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="75" customHeight="1">
+      <c r="A4" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="25" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="75.75" customHeight="1">
+      <c r="A5" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B5" s="25" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="77.25" customHeight="1">
+      <c r="A6" s="26" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>35</v>
+      <c r="B6" s="25" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="80.25" customHeight="1">
+      <c r="A7" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="25" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1153,26 +1194,6 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="21"/>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>17</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1200,7 +1221,7 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="12" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="B1" s="15" t="s">
         <v>0</v>
@@ -1209,86 +1230,86 @@
         <v>1</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="E1" s="17" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="F1" s="18" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="60">
       <c r="A2" s="4" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="45">
       <c r="A3" s="4" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="F3" s="5"/>
     </row>
     <row r="4" spans="1:6" ht="60">
       <c r="A4" s="4" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="F4" s="5"/>
     </row>
     <row r="5" spans="1:6" ht="60.75" thickBot="1">
       <c r="A5" s="6" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="F5" s="7"/>
     </row>
@@ -1419,7 +1440,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" thickBot="1">
@@ -1430,7 +1451,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -1472,7 +1493,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" thickBot="1">
@@ -1483,7 +1504,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
xml scrape unit tests
</commit_message>
<xml_diff>
--- a/DataScraperAnalysis/Spec Examples.xlsx
+++ b/DataScraperAnalysis/Spec Examples.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="15150" windowHeight="7980" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="15150" windowHeight="7980"/>
   </bookViews>
   <sheets>
     <sheet name="Scraper Error XML" sheetId="7" r:id="rId1"/>
@@ -742,7 +742,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
@@ -836,7 +836,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
scrape account adapter: telco & credit card
</commit_message>
<xml_diff>
--- a/DataScraperAnalysis/Spec Examples.xlsx
+++ b/DataScraperAnalysis/Spec Examples.xlsx
@@ -100,89 +100,6 @@
     <t>Scraper successfully scrapes a credit card company site</t>
   </si>
   <si>
-    <t>&lt;scrape-session&gt;
-  &lt;baseURL&gt;www.xbox.com&lt;/baseURL&gt;
-  &lt;date&gt;12/12/2014&lt;/date&gt;
-  &lt;time&gt;13:50:00&lt;/time&gt;
-  &lt;datapair id="001"&gt;
-    &lt;text&gt;Account Number&lt;/text&gt;
-    &lt;value&gt;123456789&lt;/value&gt;
-  &lt;/datapair&gt;
-  &lt;datapair id="002"&gt;
-    &lt;text&gt;Account holder name&lt;/text&gt;
-    &lt;value&gt;Jack Parcell&lt;/value&gt;
-  &lt;/datapair&gt;
-  &lt;datapair id="003"&gt;
-    &lt;text&gt;Statement date&lt;/text&gt;
-    &lt;value&gt;12/12/2014&lt;/value&gt;
-  &lt;/datapair&gt;
-  &lt;datapair id="004"&gt;
-    &lt;text&gt;Statement number&lt;/text&gt;
-    &lt;value&gt;1122&lt;/value&gt;
-  &lt;/datapair&gt;
-  &lt;datapair id="005"&gt;
-    &lt;text&gt;Statement month&lt;/text&gt;
-    &lt;value&gt;2&lt;/value&gt;
-  &lt;/datapair&gt;
-  &lt;datapair id="006"&gt;
-    &lt;text&gt;Total due&lt;/text&gt;
-    &lt;value&gt;R340&lt;/value&gt;
-  &lt;/datapair&gt;
-  &lt;datapair id="007"&gt;
-    &lt;text&gt;Due date&lt;/text&gt;
-    &lt;value&gt;01/01/2015&lt;/value&gt;
-  &lt;/datapair&gt;
-  &lt;datapair id="008"&gt;
-    &lt;text&gt;Opening balance&lt;/text&gt;
-    &lt;value&gt;R120&lt;/value&gt;
-  &lt;/datapair&gt;
-  &lt;datapair id="009"&gt;
-    &lt;text&gt;Closing balance&lt;/text&gt;
-    &lt;value&gt;R123&lt;/value&gt;
-  &lt;/datapair&gt;
-  &lt;datapair id="010"&gt;
-    &lt;text&gt;Payment received&lt;/text&gt;
-    &lt;value&gt;R40&lt;/value&gt;
-  &lt;/datapair&gt;
-  &lt;datapair id="011"&gt;
-    &lt;text&gt;New charges&lt;/text&gt;
-    &lt;value&gt;R45&lt;/value&gt;
-  &lt;/datapair&gt;
-  &lt;datapair id="012"&gt;
-    &lt;text&gt;Deductions&lt;/text&gt;
-    &lt;value&gt;R123&lt;/value&gt;
-  &lt;/datapair&gt;
-  &lt;datapair id="013"&gt;
-    &lt;text&gt;Discount&lt;/text&gt;
-    &lt;value&gt;R456&lt;/value&gt;
-  &lt;/datapair&gt;
-  &lt;datapair id="014"&gt;
-    &lt;text&gt;VAT Amount&lt;/text&gt;
-    &lt;value&gt;R123&lt;/value&gt;
-  &lt;/datapair&gt;
-  &lt;datapair id="015"&gt;
-    &lt;text&gt;Card type&lt;/text&gt;
-    &lt;value&gt;0721231232&lt;/value&gt;
-  &lt;/datapair&gt;
-  &lt;datapair id="016"&gt;
-    &lt;text&gt;Interest rate&lt;/text&gt;
-    &lt;value&gt;R90&lt;/value&gt;
-  &lt;/datapair&gt;
-  &lt;datapair id="017"&gt;
-    &lt;text&gt;Credit limit&lt;/text&gt;
-    &lt;value&gt;R100&lt;/value&gt;
-  &lt;/datapair&gt;
-  &lt;datapair id="018"&gt;
-    &lt;text&gt;Credit available&lt;/text&gt;
-    &lt;value&gt;R23&lt;/value&gt;
-  &lt;/datapair&gt;
-  &lt;datapair id="019"&gt;
-    &lt;text&gt;Minimum amount due&lt;/text&gt;
-    &lt;value&gt;R90&lt;/value&gt;
-  &lt;/datapair&gt;
-&lt;/scrape-session&gt;</t>
-  </si>
-  <si>
     <t>Scraper successfully scrapes a municipal site</t>
   </si>
   <si>
@@ -367,6 +284,89 @@
   &lt;/datapair&gt;
 &lt;/scrape-session&gt;
 </t>
+  </si>
+  <si>
+    <t>&lt;scrape-session&gt;_x000D_
+  &lt;baseURL&gt;www.xbox.com&lt;/baseURL&gt;_x000D_
+  &lt;date&gt;12/12/2014&lt;/date&gt;_x000D_
+  &lt;time&gt;13:50:00&lt;/time&gt;_x000D_
+  &lt;datapair id="001"&gt;_x000D_
+    &lt;text&gt;Account Number&lt;/text&gt;_x000D_
+    &lt;value&gt;123456789&lt;/value&gt;_x000D_
+  &lt;/datapair&gt;_x000D_
+  &lt;datapair id="002"&gt;_x000D_
+    &lt;text&gt;Account holder name&lt;/text&gt;_x000D_
+    &lt;value&gt;Jack Parcell&lt;/value&gt;_x000D_
+  &lt;/datapair&gt;_x000D_
+  &lt;datapair id="003"&gt;_x000D_
+    &lt;text&gt;Statement date&lt;/text&gt;_x000D_
+    &lt;value&gt;12/12/2014&lt;/value&gt;_x000D_
+  &lt;/datapair&gt;_x000D_
+  &lt;datapair id="004"&gt;_x000D_
+    &lt;text&gt;Statement number&lt;/text&gt;_x000D_
+    &lt;value&gt;1122&lt;/value&gt;_x000D_
+  &lt;/datapair&gt;_x000D_
+  &lt;datapair id="005"&gt;_x000D_
+    &lt;text&gt;Statement month&lt;/text&gt;_x000D_
+    &lt;value&gt;2&lt;/value&gt;_x000D_
+  &lt;/datapair&gt;_x000D_
+  &lt;datapair id="006"&gt;_x000D_
+    &lt;text&gt;Total due&lt;/text&gt;_x000D_
+    &lt;value&gt;R340&lt;/value&gt;_x000D_
+  &lt;/datapair&gt;_x000D_
+  &lt;datapair id="007"&gt;_x000D_
+    &lt;text&gt;Due date&lt;/text&gt;_x000D_
+    &lt;value&gt;01/01/2015&lt;/value&gt;_x000D_
+  &lt;/datapair&gt;_x000D_
+  &lt;datapair id="008"&gt;_x000D_
+    &lt;text&gt;Opening balance&lt;/text&gt;_x000D_
+    &lt;value&gt;R120&lt;/value&gt;_x000D_
+  &lt;/datapair&gt;_x000D_
+  &lt;datapair id="009"&gt;_x000D_
+    &lt;text&gt;Closing balance&lt;/text&gt;_x000D_
+    &lt;value&gt;R123&lt;/value&gt;_x000D_
+  &lt;/datapair&gt;_x000D_
+  &lt;datapair id="010"&gt;_x000D_
+    &lt;text&gt;Payment received&lt;/text&gt;_x000D_
+    &lt;value&gt;R40&lt;/value&gt;_x000D_
+  &lt;/datapair&gt;_x000D_
+  &lt;datapair id="011"&gt;_x000D_
+    &lt;text&gt;New charges&lt;/text&gt;_x000D_
+    &lt;value&gt;R45&lt;/value&gt;_x000D_
+  &lt;/datapair&gt;_x000D_
+  &lt;datapair id="012"&gt;_x000D_
+    &lt;text&gt;Deductions&lt;/text&gt;_x000D_
+    &lt;value&gt;R123&lt;/value&gt;_x000D_
+  &lt;/datapair&gt;_x000D_
+  &lt;datapair id="013"&gt;_x000D_
+    &lt;text&gt;Discount&lt;/text&gt;_x000D_
+    &lt;value&gt;R456&lt;/value&gt;_x000D_
+  &lt;/datapair&gt;_x000D_
+  &lt;datapair id="014"&gt;_x000D_
+    &lt;text&gt;VAT Amount&lt;/text&gt;_x000D_
+    &lt;value&gt;R123&lt;/value&gt;_x000D_
+  &lt;/datapair&gt;_x000D_
+  &lt;datapair id="015"&gt;_x000D_
+    &lt;text&gt;Card type&lt;/text&gt;_x000D_
+    &lt;value&gt;Visa&lt;/value&gt;_x000D_
+  &lt;/datapair&gt;_x000D_
+  &lt;datapair id="016"&gt;_x000D_
+    &lt;text&gt;Interest rate&lt;/text&gt;_x000D_
+    &lt;value&gt;12%&lt;/value&gt;_x000D_
+  &lt;/datapair&gt;_x000D_
+  &lt;datapair id="017"&gt;_x000D_
+    &lt;text&gt;Credit limit&lt;/text&gt;_x000D_
+    &lt;value&gt;R20000&lt;/value&gt;_x000D_
+  &lt;/datapair&gt;_x000D_
+  &lt;datapair id="018"&gt;_x000D_
+    &lt;text&gt;Credit available&lt;/text&gt;_x000D_
+    &lt;value&gt;R4500&lt;/value&gt;_x000D_
+  &lt;/datapair&gt;_x000D_
+  &lt;datapair id="019"&gt;_x000D_
+    &lt;text&gt;Minimum amount due&lt;/text&gt;_x000D_
+    &lt;value&gt;R90&lt;/value&gt;_x000D_
+  &lt;/datapair&gt;_x000D_
+&lt;/scrape-session&gt;</t>
   </si>
 </sst>
 </file>
@@ -425,7 +425,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -445,6 +445,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -836,8 +839,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -858,24 +861,24 @@
       <c r="A2" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>16</v>
+      <c r="B2" s="8" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="141" customHeight="1">
       <c r="A3" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>17</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="142.5" customHeight="1">
       <c r="A4" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>19</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
complete scrapeaccountadapter, complete errorxml read
</commit_message>
<xml_diff>
--- a/DataScraperAnalysis/Spec Examples.xlsx
+++ b/DataScraperAnalysis/Spec Examples.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="15150" windowHeight="7980"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="15150" windowHeight="7980" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Scraper Error XML" sheetId="7" r:id="rId1"/>
@@ -45,51 +45,7 @@
 &lt;base-url&gt;www.elen7045.co.za&lt;/base-url&gt;
 &lt;date&gt;01/06/2009&lt;/&gt;
 &lt;time&gt;12:59:34&lt;/time&gt;
-&lt;error&gt;BillingSiteDown&lt;/error&gt;
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;scrape-session&gt;
-&lt;base-url&gt;www.elen7045.co.za&lt;/base-url&gt;
-&lt;date&gt;01/06/2009&lt;/&gt;
-&lt;time&gt;12:59:34&lt;/time&gt;
-&lt;error&gt;AccountUpdateRequired&lt;/error&gt;
-&lt;/scrape-session&gt;
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;scrape-session&gt;
-&lt;base-url&gt;www.elen7045.co.za&lt;/base-url&gt;
-&lt;date&gt;01/06/2009&lt;/&gt;
-&lt;time&gt;12:59:34&lt;/time&gt;
-&lt;error&gt;InvalidCredentials&lt;/error&gt;
-&lt;/scrape-session&gt;
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;scrape-session&gt;
-&lt;base-url&gt;www.elen7045.co.za&lt;/base-url&gt;
-&lt;date&gt;01/06/2009&lt;/&gt;
-&lt;time&gt;12:59:34&lt;/time&gt;
-&lt;error&gt;UserNotSignedUpForEbilling&lt;/error&gt;
-&lt;/scrape-session&gt;
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;scrape-session&gt;
-&lt;base-url&gt;www.elen7045.co.za&lt;/base-url&gt;
-&lt;date&gt;01/06/2009&lt;/&gt;
-&lt;time&gt;12:59:34&lt;/time&gt;
 &lt;error&gt;BillingSitePageError&lt;/error&gt;
-&lt;/scrape-session&gt;
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;scrape-session&gt;
-&lt;base-url&gt;www.elen7045.co.za&lt;/base-url&gt;
-&lt;date&gt;01/06/2009&lt;/&gt;
-&lt;time&gt;12:59:34&lt;/time&gt;
-&lt;error&gt;UndeterminedError&lt;/error&gt;
 &lt;/scrape-session&gt;
 </t>
   </si>
@@ -186,6 +142,9 @@
     <t>Scraper successfully scrapes a municipal site</t>
   </si>
   <si>
+    <t>Scraper successfully scrapes a telco company site</t>
+  </si>
+  <si>
     <t xml:space="preserve">&lt;scrape-session&gt;
   &lt;baseURL&gt;www.xbox.com&lt;/baseURL&gt;
   &lt;date&gt;12/12/2014&lt;/date&gt;
@@ -247,46 +206,75 @@
     &lt;value&gt;R123&lt;/value&gt;
   &lt;/datapair&gt;
   &lt;datapair id="015"&gt;
-    &lt;text&gt;Instalment notice&lt;/text&gt;
-    &lt;value&gt;10&lt;/value&gt;
+    &lt;text&gt;Telephone number&lt;/text&gt;
+    &lt;value&gt;0721231232&lt;/value&gt;
   &lt;/datapair&gt;
   &lt;datapair id="016"&gt;
-    &lt;text&gt;Electricity used&lt;/text&gt;
-    &lt;value&gt;200kW&lt;/value&gt;
+    &lt;text&gt;Service charges&lt;/text&gt;
+    &lt;value&gt;R90&lt;/value&gt;
   &lt;/datapair&gt;
   &lt;datapair id="017"&gt;
-    &lt;text&gt;Electricity charges&lt;/text&gt;
+    &lt;text&gt;Call charges&lt;/text&gt;
     &lt;value&gt;R100&lt;/value&gt;
   &lt;/datapair&gt;
   &lt;datapair id="018"&gt;
-    &lt;text&gt;Gas used&lt;/text&gt;
-    &lt;value&gt;400Btu&lt;/value&gt;
+    &lt;text&gt;Total number of calls&lt;/text&gt;
+    &lt;value&gt;23&lt;/value&gt;
   &lt;/datapair&gt;
   &lt;datapair id="019"&gt;
-    &lt;text&gt;Water used&lt;/text&gt;
-    &lt;value&gt;300Kl&lt;/value&gt;
-  &lt;/datapair&gt;
-  &lt;datapair id="020"&gt;
-    &lt;text&gt;Water charges&lt;/text&gt;
-    &lt;value&gt;R456&lt;/value&gt;
-  &lt;/datapair&gt;
-  &lt;datapair id="021"&gt;
-    &lt;text&gt;Sewerage charges&lt;/text&gt;
-    &lt;value&gt;R345&lt;/value&gt;
-  &lt;/datapair&gt;
-  &lt;datapair id="022"&gt;
-    &lt;text&gt;Refuse charges&lt;/text&gt;
-    &lt;value&gt;R123&lt;/value&gt;
+    &lt;text&gt;Total call duration&lt;/text&gt;
+    &lt;value&gt;120mins&lt;/value&gt;
   &lt;/datapair&gt;
 &lt;/scrape-session&gt;
 </t>
   </si>
   <si>
-    <t>Scraper successfully scrapes a telco company site</t>
-  </si>
-  <si>
     <t xml:space="preserve">&lt;scrape-session&gt;
-  &lt;baseURL&gt;www.xbox.com&lt;/baseURL&gt;
+&lt;base-url&gt;www.elen7045.co.za&lt;/base-url&gt;
+&lt;date&gt;12/12/2014&lt;/&gt;
+&lt;time&gt;13:50:00&lt;/time&gt;
+&lt;error&gt;InvalidCredentials&lt;/error&gt;
+&lt;/scrape-session&gt;
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;scrape-session&gt;
+&lt;base-url&gt;www.elen7045.co.za&lt;/base-url&gt;
+&lt;date&gt;12/12/2014&lt;/&gt;
+&lt;time&gt;13:50:00&lt;/time&gt;
+&lt;error&gt;UserNotSignedUpForEbilling&lt;/error&gt;
+&lt;/scrape-session&gt;
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;scrape-session&gt;
+&lt;base-url&gt;www.elen7045.co.za&lt;/base-url&gt;
+&lt;date&gt;12/12/2014&lt;/&gt;
+&lt;time&gt;13:50:00&lt;/time&gt;
+&lt;error&gt;AccountUpdateRequired&lt;/error&gt;
+&lt;/scrape-session&gt;
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;scrape-session&gt;
+&lt;base-url&gt;www.elen7045.co.za&lt;/base-url&gt;
+&lt;date&gt;12/12/2014&lt;/&gt;
+&lt;time&gt;13:50:00&lt;/time&gt;
+&lt;error&gt;BillingSiteDown&lt;/error&gt;
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;scrape-session&gt;
+&lt;base-url&gt;www.elen7045.co.za&lt;/base-url&gt;
+&lt;date&gt;12/12/2014&lt;/&gt;
+&lt;time&gt;13:50:00&lt;/time&gt;
+&lt;error&gt;UndeterminedError&lt;/error&gt;
+&lt;/scrape-session&gt;
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;scrape-session&gt;
+  &lt;baseURL&gt;www.elen7045.co.za&lt;/baseURL&gt;
   &lt;date&gt;12/12/2014&lt;/date&gt;
   &lt;time&gt;13:50:00&lt;/time&gt;
   &lt;datapair id="001"&gt;
@@ -346,24 +334,40 @@
     &lt;value&gt;R123&lt;/value&gt;
   &lt;/datapair&gt;
   &lt;datapair id="015"&gt;
-    &lt;text&gt;Telephone number&lt;/text&gt;
-    &lt;value&gt;0721231232&lt;/value&gt;
+    &lt;text&gt;Instalment notice&lt;/text&gt;
+    &lt;value&gt;10&lt;/value&gt;
   &lt;/datapair&gt;
   &lt;datapair id="016"&gt;
-    &lt;text&gt;Service charges&lt;/text&gt;
-    &lt;value&gt;R90&lt;/value&gt;
+    &lt;text&gt;Electricity used&lt;/text&gt;
+    &lt;value&gt;200kW&lt;/value&gt;
   &lt;/datapair&gt;
   &lt;datapair id="017"&gt;
-    &lt;text&gt;Call charges&lt;/text&gt;
+    &lt;text&gt;Electricity charges&lt;/text&gt;
     &lt;value&gt;R100&lt;/value&gt;
   &lt;/datapair&gt;
   &lt;datapair id="018"&gt;
-    &lt;text&gt;Total number of calls&lt;/text&gt;
-    &lt;value&gt;23&lt;/value&gt;
+    &lt;text&gt;Gas used&lt;/text&gt;
+    &lt;value&gt;400Btu&lt;/value&gt;
   &lt;/datapair&gt;
   &lt;datapair id="019"&gt;
-    &lt;text&gt;Total call duration&lt;/text&gt;
-    &lt;value&gt;120mins&lt;/value&gt;
+    &lt;text&gt;Gas Charges&lt;/text&gt;
+    &lt;value&gt;R100&lt;/value&gt;
+  &lt;/datapair&gt;
+  &lt;datapair id="020"&gt;
+    &lt;text&gt;Water used&lt;/text&gt;
+    &lt;value&gt;300Kl&lt;/value&gt;
+  &lt;/datapair&gt;
+  &lt;datapair id="021"&gt;
+    &lt;text&gt;Water charges&lt;/text&gt;
+    &lt;value&gt;R456&lt;/value&gt;
+  &lt;/datapair&gt;
+  &lt;datapair id="022"&gt;
+    &lt;text&gt;Sewerage charges&lt;/text&gt;
+    &lt;value&gt;R345&lt;/value&gt;
+  &lt;/datapair&gt;
+  &lt;datapair id="023"&gt;
+    &lt;text&gt;Refuse charges&lt;/text&gt;
+    &lt;value&gt;R123&lt;/value&gt;
   &lt;/datapair&gt;
 &lt;/scrape-session&gt;
 </t>
@@ -742,8 +746,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -765,7 +769,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="79.5" customHeight="1">
@@ -773,7 +777,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="75" customHeight="1">
@@ -781,7 +785,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="75.75" customHeight="1">
@@ -789,7 +793,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="77.25" customHeight="1">
@@ -797,7 +801,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="80.25" customHeight="1">
@@ -805,7 +809,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -836,19 +840,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="50.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.7109375" customWidth="1"/>
+    <col min="2" max="2" width="44.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>2</v>
@@ -856,26 +860,26 @@
     </row>
     <row r="2" spans="1:2" ht="161.25" customHeight="1">
       <c r="A2" s="7" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="141" customHeight="1">
       <c r="A3" s="7" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="142.5" customHeight="1">
       <c r="A4" s="7" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
scrape exception unit test and impl complete
</commit_message>
<xml_diff>
--- a/DataScraperAnalysis/Spec Examples.xlsx
+++ b/DataScraperAnalysis/Spec Examples.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="15150" windowHeight="7980" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="15150" windowHeight="7980"/>
   </bookViews>
   <sheets>
     <sheet name="Scraper Error XML" sheetId="7" r:id="rId1"/>
@@ -41,15 +41,6 @@
     <t>Scraper attempts to scrape with a nonconforming script</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;scrape-session&gt;
-&lt;base-url&gt;www.elen7045.co.za&lt;/base-url&gt;
-&lt;date&gt;01/06/2009&lt;/&gt;
-&lt;time&gt;12:59:34&lt;/time&gt;
-&lt;error&gt;BillingSitePageError&lt;/error&gt;
-&lt;/scrape-session&gt;
-</t>
-  </si>
-  <si>
     <t>Success Scrape Scenario</t>
   </si>
   <si>
@@ -230,50 +221,6 @@
   </si>
   <si>
     <t xml:space="preserve">&lt;scrape-session&gt;
-&lt;base-url&gt;www.elen7045.co.za&lt;/base-url&gt;
-&lt;date&gt;12/12/2014&lt;/&gt;
-&lt;time&gt;13:50:00&lt;/time&gt;
-&lt;error&gt;InvalidCredentials&lt;/error&gt;
-&lt;/scrape-session&gt;
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;scrape-session&gt;
-&lt;base-url&gt;www.elen7045.co.za&lt;/base-url&gt;
-&lt;date&gt;12/12/2014&lt;/&gt;
-&lt;time&gt;13:50:00&lt;/time&gt;
-&lt;error&gt;UserNotSignedUpForEbilling&lt;/error&gt;
-&lt;/scrape-session&gt;
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;scrape-session&gt;
-&lt;base-url&gt;www.elen7045.co.za&lt;/base-url&gt;
-&lt;date&gt;12/12/2014&lt;/&gt;
-&lt;time&gt;13:50:00&lt;/time&gt;
-&lt;error&gt;AccountUpdateRequired&lt;/error&gt;
-&lt;/scrape-session&gt;
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;scrape-session&gt;
-&lt;base-url&gt;www.elen7045.co.za&lt;/base-url&gt;
-&lt;date&gt;12/12/2014&lt;/&gt;
-&lt;time&gt;13:50:00&lt;/time&gt;
-&lt;error&gt;BillingSiteDown&lt;/error&gt;
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;scrape-session&gt;
-&lt;base-url&gt;www.elen7045.co.za&lt;/base-url&gt;
-&lt;date&gt;12/12/2014&lt;/&gt;
-&lt;time&gt;13:50:00&lt;/time&gt;
-&lt;error&gt;UndeterminedError&lt;/error&gt;
-&lt;/scrape-session&gt;
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;scrape-session&gt;
   &lt;baseURL&gt;www.elen7045.co.za&lt;/baseURL&gt;
   &lt;date&gt;12/12/2014&lt;/date&gt;
   &lt;time&gt;13:50:00&lt;/time&gt;
@@ -371,6 +318,72 @@
   &lt;/datapair&gt;
 &lt;/scrape-session&gt;
 </t>
+  </si>
+  <si>
+    <t>&lt;scrape-session&gt;
+  &lt;baseURL&gt;www.elen7045.co.za&lt;/baseURL&gt;
+  &lt;date&gt;12/12/2014&lt;/date&gt;
+  &lt;time&gt;13:50:00&lt;/time&gt;
+  &lt;datapair id="001"&gt;
+    &lt;text&gt;Scraper Error&lt;/text&gt;
+    &lt;value&gt;InvalidCredentials&lt;/value&gt;
+  &lt;/datapair&gt;
+&lt;/scrape-session&gt;</t>
+  </si>
+  <si>
+    <t>&lt;scrape-session&gt;
+  &lt;baseURL&gt;www.elen7045.co.za&lt;/baseURL&gt;
+  &lt;date&gt;12/12/2014&lt;/date&gt;
+  &lt;time&gt;13:50:00&lt;/time&gt;
+  &lt;datapair id="001"&gt;
+    &lt;text&gt;Scraper Error&lt;/text&gt;
+    &lt;value&gt;UserNotSignedUpForEbilling&lt;/value&gt;
+  &lt;/datapair&gt;
+&lt;/scrape-session&gt;</t>
+  </si>
+  <si>
+    <t>&lt;scrape-session&gt;
+  &lt;baseURL&gt;www.elen7045.co.za&lt;/baseURL&gt;
+  &lt;date&gt;12/12/2014&lt;/date&gt;
+  &lt;time&gt;13:50:00&lt;/time&gt;
+  &lt;datapair id="001"&gt;
+    &lt;text&gt;Scraper Error&lt;/text&gt;
+    &lt;value&gt;AccountUpdateRequired&lt;/value&gt;
+  &lt;/datapair&gt;
+&lt;/scrape-session&gt;</t>
+  </si>
+  <si>
+    <t>&lt;scrape-session&gt;
+  &lt;baseURL&gt;www.elen7045.co.za&lt;/baseURL&gt;
+  &lt;date&gt;12/12/2014&lt;/date&gt;
+  &lt;time&gt;13:50:00&lt;/time&gt;
+  &lt;datapair id="001"&gt;
+    &lt;text&gt;Scraper Error&lt;/text&gt;
+    &lt;value&gt;BillingSiteDown&lt;/value&gt;
+  &lt;/datapair&gt;
+&lt;/scrape-session&gt;</t>
+  </si>
+  <si>
+    <t>&lt;scrape-session&gt;
+  &lt;baseURL&gt;www.elen7045.co.za&lt;/baseURL&gt;
+  &lt;date&gt;12/12/2014&lt;/date&gt;
+  &lt;time&gt;13:50:00&lt;/time&gt;
+  &lt;datapair id="001"&gt;
+    &lt;text&gt;Scraper Error&lt;/text&gt;
+    &lt;value&gt;BillingSitePageError&lt;/value&gt;
+  &lt;/datapair&gt;
+&lt;/scrape-session&gt;</t>
+  </si>
+  <si>
+    <t>&lt;scrape-session&gt;
+  &lt;baseURL&gt;www.elen7045.co.za&lt;/baseURL&gt;
+  &lt;date&gt;12/12/2014&lt;/date&gt;
+  &lt;time&gt;13:50:00&lt;/time&gt;
+  &lt;datapair id="001"&gt;
+    &lt;text&gt;Scraper Error&lt;/text&gt;
+    &lt;value&gt;UndeterminedError&lt;/value&gt;
+  &lt;/datapair&gt;
+&lt;/scrape-session&gt;</t>
   </si>
 </sst>
 </file>
@@ -744,19 +757,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="51.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="41.85546875" customWidth="1"/>
+    <col min="3" max="3" width="34.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -764,70 +778,76 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="74.25" customHeight="1">
+    <row r="2" spans="1:3" ht="151.5" customHeight="1">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="6" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="79.5" customHeight="1">
+      <c r="C2" s="6"/>
+    </row>
+    <row r="3" spans="1:3" ht="79.5" customHeight="1">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="6" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" ht="75" customHeight="1">
+      <c r="C3" s="6"/>
+    </row>
+    <row r="4" spans="1:3" ht="75" customHeight="1">
       <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" ht="75.75" customHeight="1">
+      <c r="C4" s="6"/>
+    </row>
+    <row r="5" spans="1:3" ht="75.75" customHeight="1">
       <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="6" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" ht="77.25" customHeight="1">
+      <c r="C5" s="6"/>
+    </row>
+    <row r="6" spans="1:3" ht="77.25" customHeight="1">
       <c r="A6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="80.25" customHeight="1">
+      <c r="B6" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="6"/>
+    </row>
+    <row r="7" spans="1:3" ht="80.25" customHeight="1">
       <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
+      <c r="B7" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="6"/>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" s="1"/>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:3">
       <c r="A11" s="1"/>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:3">
       <c r="A12" s="1"/>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:3">
       <c r="A13" s="1"/>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:3">
       <c r="A14" s="1"/>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:3">
       <c r="A15" s="1"/>
     </row>
   </sheetData>
@@ -840,8 +860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -852,7 +872,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>2</v>
@@ -860,26 +880,26 @@
     </row>
     <row r="2" spans="1:2" ht="161.25" customHeight="1">
       <c r="A2" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>10</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="141" customHeight="1">
       <c r="A3" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="142.5" customHeight="1">
       <c r="A4" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>13</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>